<commit_message>
changed numbers in digits to words
</commit_message>
<xml_diff>
--- a/datasets/english-french-fulfulde.xlsx
+++ b/datasets/english-french-fulfulde.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFC\PycharmProjects\no_name_for_now_dataset\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EE7F11-FC40-4ABE-B579-961F44F89255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A2E8F2-60FC-449A-812F-DEFDBD8C6594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="1160">
   <si>
     <t>English</t>
   </si>
@@ -3064,201 +3064,102 @@
     <t>stupéfait</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Go'o (if used for a single object, use 'gotel')</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Didi</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Tati</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Nay</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>Jowi</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Jowego</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>Joywe didi</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>Joywe tati</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>Joywe nye</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>Sappo</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>Sappo e go'o</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>Sappo e didi</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>Sappo e tati</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>Sappo e nye</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>Sappo e jowye</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>Sappo e jowyego</t>
   </si>
   <si>
-    <t>17</t>
-  </si>
-  <si>
     <t>Sappo e jowye didi</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
     <t>Sappo e jowye tati</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
     <t>Sappo e jowye nye</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>Nogas</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>Nogas e go'o</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>Nogas e didi</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
     <t>Nogas e nye</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>Ceppan tati</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>Ceppan nye</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>Ceppan jowye</t>
   </si>
   <si>
-    <t>60</t>
-  </si>
-  <si>
     <t>Ceppan jowyego</t>
   </si>
   <si>
-    <t>70</t>
-  </si>
-  <si>
     <t>Ceppan jowye didi</t>
   </si>
   <si>
-    <t>80</t>
-  </si>
-  <si>
     <t>Ceppan jowye tati</t>
   </si>
   <si>
-    <t>90</t>
-  </si>
-  <si>
     <t>Ceppan jowye nye</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>Temeri</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
     <t>Temeri didi</t>
   </si>
   <si>
-    <t>300</t>
-  </si>
-  <si>
     <t>Temeri tati</t>
   </si>
   <si>
@@ -3404,6 +3305,201 @@
   </si>
   <si>
     <t>vert</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">two </t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>five</t>
+  </si>
+  <si>
+    <t>six</t>
+  </si>
+  <si>
+    <t>seven</t>
+  </si>
+  <si>
+    <t>eight</t>
+  </si>
+  <si>
+    <t>nine</t>
+  </si>
+  <si>
+    <t>ten</t>
+  </si>
+  <si>
+    <t>elleven</t>
+  </si>
+  <si>
+    <t>twelve</t>
+  </si>
+  <si>
+    <t>thirteen</t>
+  </si>
+  <si>
+    <t>fourteen</t>
+  </si>
+  <si>
+    <t>fifteen</t>
+  </si>
+  <si>
+    <t>sixteen</t>
+  </si>
+  <si>
+    <t>seventeen</t>
+  </si>
+  <si>
+    <t>eighteen</t>
+  </si>
+  <si>
+    <t>nineteen</t>
+  </si>
+  <si>
+    <t>twenty</t>
+  </si>
+  <si>
+    <t>twenty-one</t>
+  </si>
+  <si>
+    <t>twenty-two</t>
+  </si>
+  <si>
+    <t>twenty-three</t>
+  </si>
+  <si>
+    <t>thirty</t>
+  </si>
+  <si>
+    <t>forty</t>
+  </si>
+  <si>
+    <t>fifty</t>
+  </si>
+  <si>
+    <t>sixty</t>
+  </si>
+  <si>
+    <t>seventy</t>
+  </si>
+  <si>
+    <t>eighty</t>
+  </si>
+  <si>
+    <t>ninety</t>
+  </si>
+  <si>
+    <t>one-hundred</t>
+  </si>
+  <si>
+    <t>two-hundred</t>
+  </si>
+  <si>
+    <t>three-hundred</t>
+  </si>
+  <si>
+    <t>un</t>
+  </si>
+  <si>
+    <t>deux</t>
+  </si>
+  <si>
+    <t>trois</t>
+  </si>
+  <si>
+    <t>quatre</t>
+  </si>
+  <si>
+    <t>cinq</t>
+  </si>
+  <si>
+    <t>sept</t>
+  </si>
+  <si>
+    <t>huit</t>
+  </si>
+  <si>
+    <t>neuf</t>
+  </si>
+  <si>
+    <t>dix</t>
+  </si>
+  <si>
+    <t>onze</t>
+  </si>
+  <si>
+    <t>douze</t>
+  </si>
+  <si>
+    <t>treize</t>
+  </si>
+  <si>
+    <t>quatorze</t>
+  </si>
+  <si>
+    <t>quinze</t>
+  </si>
+  <si>
+    <t>seize</t>
+  </si>
+  <si>
+    <t>dix-sept</t>
+  </si>
+  <si>
+    <t>dix-huit</t>
+  </si>
+  <si>
+    <t>dix-neuf</t>
+  </si>
+  <si>
+    <t>vingt</t>
+  </si>
+  <si>
+    <t>vingt et un</t>
+  </si>
+  <si>
+    <t>vingt-deux</t>
+  </si>
+  <si>
+    <t>vingt-trois</t>
+  </si>
+  <si>
+    <t>trente</t>
+  </si>
+  <si>
+    <t>quarante</t>
+  </si>
+  <si>
+    <t>cinquante</t>
+  </si>
+  <si>
+    <t>soixante</t>
+  </si>
+  <si>
+    <t>soixante-dix</t>
+  </si>
+  <si>
+    <t>quatre-vingts</t>
+  </si>
+  <si>
+    <t>quatre-vingt-dix</t>
+  </si>
+  <si>
+    <t>cent</t>
+  </si>
+  <si>
+    <t>deux cents</t>
+  </si>
+  <si>
+    <t>trois cents</t>
   </si>
 </sst>
 </file>
@@ -3768,8 +3864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
-      <selection activeCell="B432" sqref="B432"/>
+    <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
+      <selection activeCell="E405" sqref="E405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7879,541 +7975,541 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B374" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C374" t="s">
         <v>1014</v>
-      </c>
-      <c r="B374" t="s">
-        <v>1014</v>
-      </c>
-      <c r="C374" t="s">
-        <v>1015</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>1016</v>
+        <v>1096</v>
       </c>
       <c r="B375" t="s">
-        <v>1016</v>
+        <v>1129</v>
       </c>
       <c r="C375" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
-        <v>1018</v>
+        <v>1097</v>
       </c>
       <c r="B376" t="s">
-        <v>1018</v>
+        <v>1130</v>
       </c>
       <c r="C376" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>1020</v>
+        <v>1098</v>
       </c>
       <c r="B377" t="s">
-        <v>1020</v>
+        <v>1131</v>
       </c>
       <c r="C377" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>1022</v>
+        <v>1099</v>
       </c>
       <c r="B378" t="s">
-        <v>1022</v>
+        <v>1132</v>
       </c>
       <c r="C378" t="s">
-        <v>1023</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
-        <v>1024</v>
+        <v>1100</v>
       </c>
       <c r="B379" t="s">
-        <v>1024</v>
+        <v>1100</v>
       </c>
       <c r="C379" t="s">
-        <v>1025</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
-        <v>1026</v>
+        <v>1101</v>
       </c>
       <c r="B380" t="s">
-        <v>1026</v>
+        <v>1133</v>
       </c>
       <c r="C380" t="s">
-        <v>1027</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
-        <v>1028</v>
+        <v>1102</v>
       </c>
       <c r="B381" t="s">
-        <v>1028</v>
+        <v>1134</v>
       </c>
       <c r="C381" t="s">
-        <v>1029</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>1030</v>
+        <v>1103</v>
       </c>
       <c r="B382" t="s">
-        <v>1030</v>
+        <v>1135</v>
       </c>
       <c r="C382" t="s">
-        <v>1031</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
-        <v>1032</v>
+        <v>1104</v>
       </c>
       <c r="B383" t="s">
-        <v>1032</v>
+        <v>1136</v>
       </c>
       <c r="C383" t="s">
-        <v>1033</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
-        <v>1034</v>
+        <v>1105</v>
       </c>
       <c r="B384" t="s">
-        <v>1034</v>
+        <v>1137</v>
       </c>
       <c r="C384" t="s">
-        <v>1035</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
-        <v>1036</v>
+        <v>1106</v>
       </c>
       <c r="B385" t="s">
-        <v>1036</v>
+        <v>1138</v>
       </c>
       <c r="C385" t="s">
-        <v>1037</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
-        <v>1038</v>
+        <v>1107</v>
       </c>
       <c r="B386" t="s">
-        <v>1038</v>
+        <v>1139</v>
       </c>
       <c r="C386" t="s">
-        <v>1039</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
-        <v>1040</v>
+        <v>1108</v>
       </c>
       <c r="B387" t="s">
-        <v>1040</v>
+        <v>1140</v>
       </c>
       <c r="C387" t="s">
-        <v>1041</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
-        <v>1042</v>
+        <v>1109</v>
       </c>
       <c r="B388" t="s">
-        <v>1042</v>
+        <v>1141</v>
       </c>
       <c r="C388" t="s">
-        <v>1043</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
-        <v>1044</v>
+        <v>1110</v>
       </c>
       <c r="B389" t="s">
-        <v>1044</v>
+        <v>1142</v>
       </c>
       <c r="C389" t="s">
-        <v>1045</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
-        <v>1046</v>
+        <v>1111</v>
       </c>
       <c r="B390" t="s">
-        <v>1046</v>
+        <v>1143</v>
       </c>
       <c r="C390" t="s">
-        <v>1047</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
-        <v>1048</v>
+        <v>1112</v>
       </c>
       <c r="B391" t="s">
-        <v>1048</v>
+        <v>1144</v>
       </c>
       <c r="C391" t="s">
-        <v>1049</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
-        <v>1050</v>
+        <v>1113</v>
       </c>
       <c r="B392" t="s">
-        <v>1050</v>
+        <v>1145</v>
       </c>
       <c r="C392" t="s">
-        <v>1051</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>1052</v>
+        <v>1114</v>
       </c>
       <c r="B393" t="s">
-        <v>1052</v>
+        <v>1146</v>
       </c>
       <c r="C393" t="s">
-        <v>1053</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>1054</v>
+        <v>1115</v>
       </c>
       <c r="B394" t="s">
-        <v>1054</v>
+        <v>1147</v>
       </c>
       <c r="C394" t="s">
-        <v>1055</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
-        <v>1056</v>
+        <v>1116</v>
       </c>
       <c r="B395" t="s">
-        <v>1056</v>
+        <v>1148</v>
       </c>
       <c r="C395" t="s">
-        <v>1057</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
-        <v>1058</v>
+        <v>1117</v>
       </c>
       <c r="B396" t="s">
-        <v>1058</v>
+        <v>1149</v>
       </c>
       <c r="C396" t="s">
-        <v>1059</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
-        <v>1060</v>
+        <v>1118</v>
       </c>
       <c r="B397" t="s">
-        <v>1060</v>
+        <v>1150</v>
       </c>
       <c r="C397" t="s">
-        <v>1061</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
-        <v>1062</v>
+        <v>1119</v>
       </c>
       <c r="B398" t="s">
-        <v>1062</v>
+        <v>1151</v>
       </c>
       <c r="C398" t="s">
-        <v>1063</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
-        <v>1064</v>
+        <v>1120</v>
       </c>
       <c r="B399" t="s">
-        <v>1064</v>
+        <v>1152</v>
       </c>
       <c r="C399" t="s">
-        <v>1065</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
-        <v>1066</v>
+        <v>1121</v>
       </c>
       <c r="B400" t="s">
-        <v>1066</v>
+        <v>1153</v>
       </c>
       <c r="C400" t="s">
-        <v>1067</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
-        <v>1068</v>
+        <v>1122</v>
       </c>
       <c r="B401" t="s">
-        <v>1068</v>
+        <v>1154</v>
       </c>
       <c r="C401" t="s">
-        <v>1069</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
-        <v>1070</v>
+        <v>1123</v>
       </c>
       <c r="B402" t="s">
-        <v>1070</v>
+        <v>1155</v>
       </c>
       <c r="C402" t="s">
-        <v>1071</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
-        <v>1072</v>
+        <v>1124</v>
       </c>
       <c r="B403" t="s">
-        <v>1072</v>
+        <v>1156</v>
       </c>
       <c r="C403" t="s">
-        <v>1073</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
-        <v>1074</v>
+        <v>1125</v>
       </c>
       <c r="B404" t="s">
-        <v>1074</v>
+        <v>1157</v>
       </c>
       <c r="C404" t="s">
-        <v>1075</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
-        <v>1076</v>
+        <v>1126</v>
       </c>
       <c r="B405" t="s">
-        <v>1076</v>
+        <v>1158</v>
       </c>
       <c r="C405" t="s">
-        <v>1077</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
-        <v>1078</v>
+        <v>1127</v>
       </c>
       <c r="B406" t="s">
-        <v>1078</v>
+        <v>1159</v>
       </c>
       <c r="C406" t="s">
-        <v>1079</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
-        <v>1080</v>
+        <v>1047</v>
       </c>
       <c r="B407" t="s">
-        <v>1082</v>
+        <v>1049</v>
       </c>
       <c r="C407" t="s">
-        <v>1081</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
-        <v>1083</v>
+        <v>1050</v>
       </c>
       <c r="B408" t="s">
-        <v>1085</v>
+        <v>1052</v>
       </c>
       <c r="C408" t="s">
-        <v>1084</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
-        <v>1086</v>
+        <v>1053</v>
       </c>
       <c r="B409" t="s">
-        <v>1088</v>
+        <v>1055</v>
       </c>
       <c r="C409" t="s">
-        <v>1087</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
-        <v>1089</v>
+        <v>1056</v>
       </c>
       <c r="B410" t="s">
-        <v>1091</v>
+        <v>1058</v>
       </c>
       <c r="C410" t="s">
-        <v>1090</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
-        <v>1092</v>
+        <v>1059</v>
       </c>
       <c r="B411" t="s">
-        <v>1094</v>
+        <v>1061</v>
       </c>
       <c r="C411" t="s">
-        <v>1093</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
-        <v>1095</v>
+        <v>1062</v>
       </c>
       <c r="B412" t="s">
-        <v>1097</v>
+        <v>1064</v>
       </c>
       <c r="C412" t="s">
-        <v>1096</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
-        <v>1098</v>
+        <v>1065</v>
       </c>
       <c r="B413" t="s">
-        <v>1100</v>
+        <v>1067</v>
       </c>
       <c r="C413" t="s">
-        <v>1099</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
-        <v>1101</v>
+        <v>1068</v>
       </c>
       <c r="B414" t="s">
-        <v>1103</v>
+        <v>1070</v>
       </c>
       <c r="C414" t="s">
-        <v>1102</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
-        <v>1104</v>
+        <v>1071</v>
       </c>
       <c r="B415" t="s">
-        <v>1106</v>
+        <v>1073</v>
       </c>
       <c r="C415" t="s">
-        <v>1105</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
-        <v>1107</v>
+        <v>1074</v>
       </c>
       <c r="B416" t="s">
-        <v>1109</v>
+        <v>1076</v>
       </c>
       <c r="C416" t="s">
-        <v>1108</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
-        <v>1110</v>
+        <v>1077</v>
       </c>
       <c r="B417" t="s">
-        <v>1112</v>
+        <v>1079</v>
       </c>
       <c r="C417" t="s">
-        <v>1111</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
-        <v>1113</v>
+        <v>1080</v>
       </c>
       <c r="B418" t="s">
-        <v>1115</v>
+        <v>1082</v>
       </c>
       <c r="C418" t="s">
-        <v>1114</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
-        <v>1116</v>
+        <v>1083</v>
       </c>
       <c r="B419" t="s">
-        <v>1118</v>
+        <v>1085</v>
       </c>
       <c r="C419" t="s">
-        <v>1117</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
-        <v>1119</v>
+        <v>1086</v>
       </c>
       <c r="B420" t="s">
-        <v>1121</v>
+        <v>1088</v>
       </c>
       <c r="C420" t="s">
-        <v>1120</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
-        <v>1122</v>
+        <v>1089</v>
       </c>
       <c r="B421" t="s">
-        <v>1124</v>
+        <v>1091</v>
       </c>
       <c r="C421" t="s">
-        <v>1123</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
-        <v>1125</v>
+        <v>1092</v>
       </c>
       <c r="B422" t="s">
-        <v>1127</v>
+        <v>1094</v>
       </c>
       <c r="C422" t="s">
-        <v>1126</v>
+        <v>1093</v>
       </c>
     </row>
   </sheetData>

</xml_diff>